<commit_message>
Updated db pragmas to enable foreign keys
</commit_message>
<xml_diff>
--- a/tests/sample_input_data_missing_data.xlsx
+++ b/tests/sample_input_data_missing_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="223">
   <si>
     <t>OD600</t>
   </si>
@@ -1011,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O208"/>
+  <dimension ref="A1:O207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="B173" sqref="B173"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156:XFD156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8303,10 +8303,10 @@
     </row>
     <row r="156" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B156">
-        <v>0</v>
+        <v>28.428714999344336</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -8330,7 +8330,7 @@
         <v>0</v>
       </c>
       <c r="J156">
-        <v>0</v>
+        <v>2.726287652875584E-2</v>
       </c>
       <c r="K156">
         <v>0</v>
@@ -8345,18 +8345,18 @@
         <v>0</v>
       </c>
       <c r="O156">
-        <v>0.24271500306581498</v>
+        <v>0.45999899419884321</v>
       </c>
     </row>
     <row r="157" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B157">
-        <v>28.428714999344336</v>
+        <v>27.200904529975315</v>
       </c>
       <c r="C157">
-        <v>0</v>
+        <v>2.3194275420636984E-2</v>
       </c>
       <c r="D157">
         <v>0</v>
@@ -8371,13 +8371,13 @@
         <v>0</v>
       </c>
       <c r="H157">
-        <v>0</v>
+        <v>0.35184558844183789</v>
       </c>
       <c r="I157">
         <v>0</v>
       </c>
       <c r="J157">
-        <v>2.726287652875584E-2</v>
+        <v>0.16501394246602413</v>
       </c>
       <c r="K157">
         <v>0</v>
@@ -8386,24 +8386,24 @@
         <v>0</v>
       </c>
       <c r="M157">
-        <v>0</v>
+        <v>9.7595868293103485E-3</v>
       </c>
       <c r="N157">
         <v>0</v>
       </c>
       <c r="O157">
-        <v>0.45999899419884321</v>
+        <v>0.92715936065265681</v>
       </c>
     </row>
     <row r="158" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B158">
-        <v>27.200904529975315</v>
+        <v>25.356899168007505</v>
       </c>
       <c r="C158">
-        <v>2.3194275420636984E-2</v>
+        <v>3.7394708712119348E-2</v>
       </c>
       <c r="D158">
         <v>0</v>
@@ -8418,39 +8418,39 @@
         <v>0</v>
       </c>
       <c r="H158">
-        <v>0.35184558844183789</v>
+        <v>0.57315051155429564</v>
       </c>
       <c r="I158">
         <v>0</v>
       </c>
       <c r="J158">
-        <v>0.16501394246602413</v>
+        <v>0.23631739209385585</v>
       </c>
       <c r="K158">
-        <v>0</v>
+        <v>2.9176551639578614E-2</v>
       </c>
       <c r="L158">
-        <v>0</v>
+        <v>3.2566203004239401E-3</v>
       </c>
       <c r="M158">
-        <v>9.7595868293103485E-3</v>
+        <v>4.1900964437695705E-2</v>
       </c>
       <c r="N158">
         <v>0</v>
       </c>
       <c r="O158">
-        <v>0.92715936065265681</v>
+        <v>1.6885900555849649</v>
       </c>
     </row>
     <row r="159" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B159">
-        <v>25.356899168007505</v>
+        <v>23.396581149221191</v>
       </c>
       <c r="C159">
-        <v>3.7394708712119348E-2</v>
+        <v>0.15147861040650673</v>
       </c>
       <c r="D159">
         <v>0</v>
@@ -8465,39 +8465,39 @@
         <v>0</v>
       </c>
       <c r="H159">
-        <v>0.57315051155429564</v>
+        <v>0.67742805507862303</v>
       </c>
       <c r="I159">
         <v>0</v>
       </c>
       <c r="J159">
-        <v>0.23631739209385585</v>
+        <v>0.13765781564389049</v>
       </c>
       <c r="K159">
-        <v>2.9176551639578614E-2</v>
+        <v>7.4376225565992535E-2</v>
       </c>
       <c r="L159">
-        <v>3.2566203004239401E-3</v>
+        <v>0</v>
       </c>
       <c r="M159">
-        <v>4.1900964437695705E-2</v>
+        <v>6.715061898745428E-2</v>
       </c>
       <c r="N159">
         <v>0</v>
       </c>
       <c r="O159">
-        <v>1.6885900555849649</v>
+        <v>3.2453715503303222</v>
       </c>
     </row>
     <row r="160" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B160">
-        <v>23.396581149221191</v>
+        <v>19.123391170397039</v>
       </c>
       <c r="C160">
-        <v>0.15147861040650673</v>
+        <v>0.22044856533244453</v>
       </c>
       <c r="D160">
         <v>0</v>
@@ -8512,39 +8512,39 @@
         <v>0</v>
       </c>
       <c r="H160">
-        <v>0.67742805507862303</v>
+        <v>0.90097288129749364</v>
       </c>
       <c r="I160">
-        <v>0</v>
+        <v>0.22298525325447888</v>
       </c>
       <c r="J160">
-        <v>0.13765781564389049</v>
+        <v>0.62292391253612345</v>
       </c>
       <c r="K160">
-        <v>7.4376225565992535E-2</v>
+        <v>0.47053141264429638</v>
       </c>
       <c r="L160">
-        <v>0</v>
+        <v>0.29426919542705671</v>
       </c>
       <c r="M160">
-        <v>6.715061898745428E-2</v>
+        <v>0.43589093801904455</v>
       </c>
       <c r="N160">
         <v>0</v>
       </c>
       <c r="O160">
-        <v>3.2453715503303222</v>
+        <v>5.3771826439194639</v>
       </c>
     </row>
     <row r="161" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B161">
-        <v>19.123391170397039</v>
+        <v>42.783204465354039</v>
       </c>
       <c r="C161">
-        <v>0.22044856533244453</v>
+        <v>0.24600848188806509</v>
       </c>
       <c r="D161">
         <v>0</v>
@@ -8559,39 +8559,39 @@
         <v>0</v>
       </c>
       <c r="H161">
-        <v>0.90097288129749364</v>
+        <v>0.67618279976736495</v>
       </c>
       <c r="I161">
-        <v>0.22298525325447888</v>
+        <v>0.19958484636962875</v>
       </c>
       <c r="J161">
-        <v>0.62292391253612345</v>
+        <v>0.54757901609918891</v>
       </c>
       <c r="K161">
-        <v>0.47053141264429638</v>
+        <v>0.27363402237938828</v>
       </c>
       <c r="L161">
-        <v>0.29426919542705671</v>
+        <v>0.31264928530811215</v>
       </c>
       <c r="M161">
-        <v>0.43589093801904455</v>
+        <v>0.3823367219605166</v>
       </c>
       <c r="N161">
         <v>0</v>
       </c>
       <c r="O161">
-        <v>5.3771826439194639</v>
+        <v>5.3391426026155697</v>
       </c>
     </row>
     <row r="162" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B162">
-        <v>42.783204465354039</v>
+        <v>47.920212511415421</v>
       </c>
       <c r="C162">
-        <v>0.24600848188806509</v>
+        <v>9.1217194055802905E-2</v>
       </c>
       <c r="D162">
         <v>0</v>
@@ -8606,39 +8606,39 @@
         <v>0</v>
       </c>
       <c r="H162">
-        <v>0.67618279976736495</v>
+        <v>0.98361781929505232</v>
       </c>
       <c r="I162">
-        <v>0.19958484636962875</v>
+        <v>0.47000321694098085</v>
       </c>
       <c r="J162">
-        <v>0.54757901609918891</v>
+        <v>0.85482086102183696</v>
       </c>
       <c r="K162">
-        <v>0.27363402237938828</v>
+        <v>1.081963864735378</v>
       </c>
       <c r="L162">
-        <v>0.31264928530811215</v>
+        <v>0.72472784577067695</v>
       </c>
       <c r="M162">
-        <v>0.3823367219605166</v>
+        <v>0.90401492777822556</v>
       </c>
       <c r="N162">
         <v>0</v>
       </c>
       <c r="O162">
-        <v>5.3391426026155697</v>
+        <v>5.2184680356032844</v>
       </c>
     </row>
     <row r="163" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B163">
-        <v>47.920212511415421</v>
+        <v>46.048973750927189</v>
       </c>
       <c r="C163">
-        <v>9.1217194055802905E-2</v>
+        <v>0</v>
       </c>
       <c r="D163">
         <v>0</v>
@@ -8653,36 +8653,36 @@
         <v>0</v>
       </c>
       <c r="H163">
-        <v>0.98361781929505232</v>
+        <v>0.87673657781166003</v>
       </c>
       <c r="I163">
-        <v>0.47000321694098085</v>
+        <v>0.58119319898662003</v>
       </c>
       <c r="J163">
-        <v>0.85482086102183696</v>
+        <v>0.97794648380310312</v>
       </c>
       <c r="K163">
-        <v>1.081963864735378</v>
+        <v>0.75497497331767338</v>
       </c>
       <c r="L163">
-        <v>0.72472784577067695</v>
+        <v>0.86782128591369168</v>
       </c>
       <c r="M163">
-        <v>0.90401492777822556</v>
+        <v>1.465438824242689</v>
       </c>
       <c r="N163">
         <v>0</v>
       </c>
       <c r="O163">
-        <v>5.2184680356032844</v>
+        <v>4.4579247848171839</v>
       </c>
     </row>
     <row r="164" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B164">
-        <v>46.048973750927189</v>
+        <v>36.696837326347733</v>
       </c>
       <c r="C164">
         <v>0</v>
@@ -8700,36 +8700,36 @@
         <v>0</v>
       </c>
       <c r="H164">
-        <v>0.87673657781166003</v>
+        <v>0.95887521857248792</v>
       </c>
       <c r="I164">
-        <v>0.58119319898662003</v>
+        <v>0.81313389137089043</v>
       </c>
       <c r="J164">
-        <v>0.97794648380310312</v>
+        <v>1.1860794618816508</v>
       </c>
       <c r="K164">
-        <v>0.75497497331767338</v>
+        <v>0.89344478998205445</v>
       </c>
       <c r="L164">
-        <v>0.86782128591369168</v>
+        <v>0.85834942842389161</v>
       </c>
       <c r="M164">
-        <v>1.465438824242689</v>
+        <v>2.0941326583293982</v>
       </c>
       <c r="N164">
         <v>0</v>
       </c>
       <c r="O164">
-        <v>4.4579247848171839</v>
+        <v>4.3770611569154791</v>
       </c>
     </row>
     <row r="165" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B165">
-        <v>36.696837326347733</v>
+        <v>0</v>
       </c>
       <c r="C165">
         <v>0</v>
@@ -8747,36 +8747,36 @@
         <v>0</v>
       </c>
       <c r="H165">
-        <v>0.95887521857248792</v>
+        <v>0</v>
       </c>
       <c r="I165">
-        <v>0.81313389137089043</v>
+        <v>0</v>
       </c>
       <c r="J165">
-        <v>1.1860794618816508</v>
+        <v>0</v>
       </c>
       <c r="K165">
-        <v>0.89344478998205445</v>
+        <v>0</v>
       </c>
       <c r="L165">
-        <v>0.85834942842389161</v>
+        <v>0</v>
       </c>
       <c r="M165">
-        <v>2.0941326583293982</v>
+        <v>0</v>
       </c>
       <c r="N165">
         <v>0</v>
       </c>
       <c r="O165">
-        <v>4.3770611569154791</v>
+        <v>0.19839558540886784</v>
       </c>
     </row>
     <row r="166" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B166">
-        <v>0</v>
+        <v>26.210711440416187</v>
       </c>
       <c r="C166">
         <v>0</v>
@@ -8800,7 +8800,7 @@
         <v>0</v>
       </c>
       <c r="J166">
-        <v>0</v>
+        <v>2.2828721062786262E-2</v>
       </c>
       <c r="K166">
         <v>0</v>
@@ -8815,18 +8815,18 @@
         <v>0</v>
       </c>
       <c r="O166">
-        <v>0.19839558540886784</v>
+        <v>0.50879774293282409</v>
       </c>
     </row>
     <row r="167" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B167">
-        <v>26.210711440416187</v>
+        <v>30.488156600878433</v>
       </c>
       <c r="C167">
-        <v>0</v>
+        <v>2.8689321614988109E-2</v>
       </c>
       <c r="D167">
         <v>0</v>
@@ -8841,13 +8841,13 @@
         <v>0</v>
       </c>
       <c r="H167">
-        <v>0</v>
+        <v>0.43122666288151518</v>
       </c>
       <c r="I167">
         <v>0</v>
       </c>
       <c r="J167">
-        <v>2.2828721062786262E-2</v>
+        <v>0.15478889768656159</v>
       </c>
       <c r="K167">
         <v>0</v>
@@ -8862,18 +8862,18 @@
         <v>0</v>
       </c>
       <c r="O167">
-        <v>0.50879774293282409</v>
+        <v>1.264799702961529</v>
       </c>
     </row>
     <row r="168" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B168">
-        <v>30.488156600878433</v>
+        <v>27.166575315254747</v>
       </c>
       <c r="C168">
-        <v>2.8689321614988109E-2</v>
+        <v>5.6610460511909183E-2</v>
       </c>
       <c r="D168">
         <v>0</v>
@@ -8888,39 +8888,39 @@
         <v>0</v>
       </c>
       <c r="H168">
-        <v>0.43122666288151518</v>
+        <v>0.57646630540589217</v>
       </c>
       <c r="I168">
         <v>0</v>
       </c>
       <c r="J168">
-        <v>0.15478889768656159</v>
+        <v>0.23777615957797937</v>
       </c>
       <c r="K168">
-        <v>0</v>
+        <v>3.2079268871719364E-2</v>
       </c>
       <c r="L168">
         <v>0</v>
       </c>
       <c r="M168">
-        <v>0</v>
+        <v>5.2654594269875191E-2</v>
       </c>
       <c r="N168">
         <v>0</v>
       </c>
       <c r="O168">
-        <v>1.264799702961529</v>
+        <v>2.3560223866467136</v>
       </c>
     </row>
     <row r="169" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B169">
-        <v>27.166575315254747</v>
+        <v>24.785949276769905</v>
       </c>
       <c r="C169">
-        <v>5.6610460511909183E-2</v>
+        <v>0.15703367867823609</v>
       </c>
       <c r="D169">
         <v>0</v>
@@ -8935,39 +8935,39 @@
         <v>0</v>
       </c>
       <c r="H169">
-        <v>0.57646630540589217</v>
+        <v>0.84470930262009747</v>
       </c>
       <c r="I169">
         <v>0</v>
       </c>
       <c r="J169">
-        <v>0.23777615957797937</v>
+        <v>0.13526230526909322</v>
       </c>
       <c r="K169">
-        <v>3.2079268871719364E-2</v>
+        <v>9.8090908726610471E-2</v>
       </c>
       <c r="L169">
         <v>0</v>
       </c>
       <c r="M169">
-        <v>5.2654594269875191E-2</v>
+        <v>0.11901854856539847</v>
       </c>
       <c r="N169">
         <v>0</v>
       </c>
       <c r="O169">
-        <v>2.3560223866467136</v>
+        <v>4.0108155464101882</v>
       </c>
     </row>
     <row r="170" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B170">
-        <v>24.785949276769905</v>
+        <v>14.020345630622408</v>
       </c>
       <c r="C170">
-        <v>0.15703367867823609</v>
+        <v>0.18338333956402442</v>
       </c>
       <c r="D170">
         <v>0</v>
@@ -8982,39 +8982,39 @@
         <v>0</v>
       </c>
       <c r="H170">
-        <v>0.84470930262009747</v>
+        <v>0.86937005453584748</v>
       </c>
       <c r="I170">
-        <v>0</v>
+        <v>0.23818354381210421</v>
       </c>
       <c r="J170">
-        <v>0.13526230526909322</v>
+        <v>0.77063603233654498</v>
       </c>
       <c r="K170">
-        <v>9.8090908726610471E-2</v>
+        <v>0.4928697060431429</v>
       </c>
       <c r="L170">
-        <v>0</v>
+        <v>0.64416526185391954</v>
       </c>
       <c r="M170">
-        <v>0.11901854856539847</v>
+        <v>0.5069068947054588</v>
       </c>
       <c r="N170">
         <v>0</v>
       </c>
       <c r="O170">
-        <v>4.0108155464101882</v>
+        <v>6.0576031542629982</v>
       </c>
     </row>
     <row r="171" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B171">
-        <v>14.020345630622408</v>
+        <v>41.963513241641017</v>
       </c>
       <c r="C171">
-        <v>0.18338333956402442</v>
+        <v>0.20977635404843351</v>
       </c>
       <c r="D171">
         <v>0</v>
@@ -9029,39 +9029,39 @@
         <v>0</v>
       </c>
       <c r="H171">
-        <v>0.86937005453584748</v>
+        <v>0.74393685810075749</v>
       </c>
       <c r="I171">
-        <v>0.23818354381210421</v>
+        <v>0.22150348127025926</v>
       </c>
       <c r="J171">
-        <v>0.77063603233654498</v>
+        <v>0.72077960948721165</v>
       </c>
       <c r="K171">
-        <v>0.4928697060431429</v>
+        <v>0.45079457485114444</v>
       </c>
       <c r="L171">
-        <v>0.64416526185391954</v>
+        <v>0.62622872466825497</v>
       </c>
       <c r="M171">
-        <v>0.5069068947054588</v>
+        <v>0.52686595545976</v>
       </c>
       <c r="N171">
         <v>0</v>
       </c>
       <c r="O171">
-        <v>6.0576031542629982</v>
+        <v>5.7115012870102415</v>
       </c>
     </row>
     <row r="172" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B172">
-        <v>41.963513241641017</v>
+        <v>39.499278943357439</v>
       </c>
       <c r="C172">
-        <v>0.20977635404843351</v>
+        <v>2.1820076099513093E-2</v>
       </c>
       <c r="D172">
         <v>0</v>
@@ -9076,39 +9076,39 @@
         <v>0</v>
       </c>
       <c r="H172">
-        <v>0.74393685810075749</v>
+        <v>0.94208939986753792</v>
       </c>
       <c r="I172">
-        <v>0.22150348127025926</v>
+        <v>0.45025135263218713</v>
       </c>
       <c r="J172">
-        <v>0.72077960948721165</v>
+        <v>0.70218171636319726</v>
       </c>
       <c r="K172">
-        <v>0.45079457485114444</v>
+        <v>0.79743096556173865</v>
       </c>
       <c r="L172">
-        <v>0.62622872466825497</v>
+        <v>1.0808986028628471</v>
       </c>
       <c r="M172">
-        <v>0.52686595545976</v>
+        <v>0.88166297696335316</v>
       </c>
       <c r="N172">
         <v>0</v>
       </c>
       <c r="O172">
-        <v>5.7115012870102415</v>
+        <v>5.9502650635308214</v>
       </c>
     </row>
     <row r="173" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B173">
-        <v>39.499278943357439</v>
+        <v>35.691159213772508</v>
       </c>
       <c r="C173">
-        <v>2.1820076099513093E-2</v>
+        <v>0</v>
       </c>
       <c r="D173">
         <v>0</v>
@@ -9123,36 +9123,36 @@
         <v>0</v>
       </c>
       <c r="H173">
-        <v>0.94208939986753792</v>
+        <v>0.92179866292826851</v>
       </c>
       <c r="I173">
-        <v>0.45025135263218713</v>
+        <v>0.59413649814594571</v>
       </c>
       <c r="J173">
-        <v>0.70218171636319726</v>
+        <v>0.57995649991007026</v>
       </c>
       <c r="K173">
-        <v>0.79743096556173865</v>
+        <v>0.98469838109258723</v>
       </c>
       <c r="L173">
-        <v>1.0808986028628471</v>
+        <v>1.5691838706186596</v>
       </c>
       <c r="M173">
-        <v>0.88166297696335316</v>
+        <v>1.192902617256095</v>
       </c>
       <c r="N173">
         <v>0</v>
       </c>
       <c r="O173">
-        <v>5.9502650635308214</v>
+        <v>5.5225275359599904</v>
       </c>
     </row>
     <row r="174" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B174">
-        <v>35.691159213772508</v>
+        <v>39.262442284367303</v>
       </c>
       <c r="C174">
         <v>0</v>
@@ -9170,36 +9170,36 @@
         <v>0</v>
       </c>
       <c r="H174">
-        <v>0.92179866292826851</v>
+        <v>0.87485561878762985</v>
       </c>
       <c r="I174">
-        <v>0.59413649814594571</v>
+        <v>0.82810782726369692</v>
       </c>
       <c r="J174">
-        <v>0.57995649991007026</v>
+        <v>0.57024439837900442</v>
       </c>
       <c r="K174">
-        <v>0.98469838109258723</v>
+        <v>1.2762860100959026</v>
       </c>
       <c r="L174">
-        <v>1.5691838706186596</v>
+        <v>2.1067085510888228</v>
       </c>
       <c r="M174">
-        <v>1.192902617256095</v>
+        <v>1.5909530600597361</v>
       </c>
       <c r="N174">
         <v>0</v>
       </c>
       <c r="O174">
-        <v>5.5225275359599904</v>
+        <v>4.8295154702838037</v>
       </c>
     </row>
     <row r="175" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
-        <v>130</v>
+        <v>189</v>
       </c>
       <c r="B175">
-        <v>39.262442284367303</v>
+        <v>0</v>
       </c>
       <c r="C175">
         <v>0</v>
@@ -9217,33 +9217,33 @@
         <v>0</v>
       </c>
       <c r="H175">
-        <v>0.87485561878762985</v>
+        <v>0</v>
       </c>
       <c r="I175">
-        <v>0.82810782726369692</v>
+        <v>0</v>
       </c>
       <c r="J175">
-        <v>0.57024439837900442</v>
+        <v>0</v>
       </c>
       <c r="K175">
-        <v>1.2762860100959026</v>
+        <v>0</v>
       </c>
       <c r="L175">
-        <v>2.1067085510888228</v>
+        <v>0</v>
       </c>
       <c r="M175">
-        <v>1.5909530600597361</v>
+        <v>0</v>
       </c>
       <c r="N175">
         <v>0</v>
       </c>
       <c r="O175">
-        <v>4.8295154702838037</v>
+        <v>0.16602462016966377</v>
       </c>
     </row>
     <row r="176" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B176">
         <v>0</v>
@@ -9285,15 +9285,15 @@
         <v>0</v>
       </c>
       <c r="O176">
-        <v>0.16602462016966377</v>
+        <v>0.20677910561152099</v>
       </c>
     </row>
     <row r="177" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B177">
-        <v>0</v>
+        <v>32.616358749104343</v>
       </c>
       <c r="C177">
         <v>0</v>
@@ -9332,18 +9332,18 @@
         <v>0</v>
       </c>
       <c r="O177">
-        <v>0.20677910561152099</v>
+        <v>0.23527309636057306</v>
       </c>
     </row>
     <row r="178" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B178">
-        <v>32.616358749104343</v>
+        <v>31.792176921235782</v>
       </c>
       <c r="C178">
-        <v>0</v>
+        <v>1.410715185241304E-2</v>
       </c>
       <c r="D178">
         <v>0</v>
@@ -9358,7 +9358,7 @@
         <v>0</v>
       </c>
       <c r="H178">
-        <v>0</v>
+        <v>0.31836657709076677</v>
       </c>
       <c r="I178">
         <v>0</v>
@@ -9379,18 +9379,18 @@
         <v>0</v>
       </c>
       <c r="O178">
-        <v>0.23527309636057306</v>
+        <v>0.72329210403087296</v>
       </c>
     </row>
     <row r="179" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B179">
-        <v>31.792176921235782</v>
+        <v>30.471930695350832</v>
       </c>
       <c r="C179">
-        <v>1.410715185241304E-2</v>
+        <v>0.10427530425080749</v>
       </c>
       <c r="D179">
         <v>0</v>
@@ -9405,7 +9405,7 @@
         <v>0</v>
       </c>
       <c r="H179">
-        <v>0.31836657709076677</v>
+        <v>0.48870582503369758</v>
       </c>
       <c r="I179">
         <v>0</v>
@@ -9426,18 +9426,18 @@
         <v>0</v>
       </c>
       <c r="O179">
-        <v>0.72329210403087296</v>
+        <v>1.0103885507437727</v>
       </c>
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B180">
-        <v>30.471930695350832</v>
+        <v>28.753646018813022</v>
       </c>
       <c r="C180">
-        <v>0.10427530425080749</v>
+        <v>0.26638251944622743</v>
       </c>
       <c r="D180">
         <v>0</v>
@@ -9452,7 +9452,7 @@
         <v>0</v>
       </c>
       <c r="H180">
-        <v>0.48870582503369758</v>
+        <v>0.74379670380513963</v>
       </c>
       <c r="I180">
         <v>0</v>
@@ -9473,18 +9473,18 @@
         <v>0</v>
       </c>
       <c r="O180">
-        <v>1.0103885507437727</v>
+        <v>1.9422793832149141</v>
       </c>
     </row>
     <row r="181" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B181">
-        <v>28.753646018813022</v>
+        <v>22.41298740226209</v>
       </c>
       <c r="C181">
-        <v>0.26638251944622743</v>
+        <v>2.4343643720729444</v>
       </c>
       <c r="D181">
         <v>0</v>
@@ -9499,39 +9499,39 @@
         <v>0</v>
       </c>
       <c r="H181">
-        <v>0.74379670380513963</v>
+        <v>1.2847232941500739</v>
       </c>
       <c r="I181">
         <v>0</v>
       </c>
       <c r="J181">
-        <v>0</v>
+        <v>0.13139754741925555</v>
       </c>
       <c r="K181">
-        <v>0</v>
+        <v>0.12009656288557986</v>
       </c>
       <c r="L181">
         <v>0</v>
       </c>
       <c r="M181">
-        <v>0</v>
+        <v>6.3021792900221557E-2</v>
       </c>
       <c r="N181">
         <v>0</v>
       </c>
       <c r="O181">
-        <v>1.9422793832149141</v>
+        <v>3.8164516610272159</v>
       </c>
     </row>
     <row r="182" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B182">
-        <v>22.41298740226209</v>
+        <v>53.010937290234956</v>
       </c>
       <c r="C182">
-        <v>2.4343643720729444</v>
+        <v>2.2158903285670415</v>
       </c>
       <c r="D182">
         <v>0</v>
@@ -9546,39 +9546,39 @@
         <v>0</v>
       </c>
       <c r="H182">
-        <v>1.2847232941500739</v>
+        <v>1.0403520318772559</v>
       </c>
       <c r="I182">
-        <v>0</v>
+        <v>3.627948667444101E-2</v>
       </c>
       <c r="J182">
-        <v>0.13139754741925555</v>
+        <v>0.15182150415655774</v>
       </c>
       <c r="K182">
-        <v>0.12009656288557986</v>
+        <v>6.7148749867230462E-2</v>
       </c>
       <c r="L182">
         <v>0</v>
       </c>
       <c r="M182">
-        <v>6.3021792900221557E-2</v>
+        <v>8.4644147124556646E-2</v>
       </c>
       <c r="N182">
         <v>0</v>
       </c>
       <c r="O182">
-        <v>3.8164516610272159</v>
+        <v>3.9405828508351712</v>
       </c>
     </row>
     <row r="183" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B183">
-        <v>53.010937290234956</v>
+        <v>49.96808204821275</v>
       </c>
       <c r="C183">
-        <v>2.2158903285670415</v>
+        <v>2.7414624641218666</v>
       </c>
       <c r="D183">
         <v>0</v>
@@ -9593,39 +9593,39 @@
         <v>0</v>
       </c>
       <c r="H183">
-        <v>1.0403520318772559</v>
+        <v>1.5115449770283393</v>
       </c>
       <c r="I183">
-        <v>3.627948667444101E-2</v>
+        <v>0.19532612254220363</v>
       </c>
       <c r="J183">
-        <v>0.15182150415655774</v>
+        <v>0.18825254469307492</v>
       </c>
       <c r="K183">
-        <v>6.7148749867230462E-2</v>
+        <v>0.12049851899967801</v>
       </c>
       <c r="L183">
         <v>0</v>
       </c>
       <c r="M183">
-        <v>8.4644147124556646E-2</v>
+        <v>0.22782175671685601</v>
       </c>
       <c r="N183">
         <v>0</v>
       </c>
       <c r="O183">
-        <v>3.9405828508351712</v>
+        <v>4.8791799471685291</v>
       </c>
     </row>
     <row r="184" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A184" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B184">
-        <v>49.96808204821275</v>
+        <v>46.21755826388241</v>
       </c>
       <c r="C184">
-        <v>2.7414624641218666</v>
+        <v>1.8551334779896211</v>
       </c>
       <c r="D184">
         <v>0</v>
@@ -9640,39 +9640,39 @@
         <v>0</v>
       </c>
       <c r="H184">
-        <v>1.5115449770283393</v>
+        <v>2.0743997343479981</v>
       </c>
       <c r="I184">
-        <v>0.19532612254220363</v>
+        <v>0.35315276067282059</v>
       </c>
       <c r="J184">
-        <v>0.18825254469307492</v>
+        <v>0.22087448275496138</v>
       </c>
       <c r="K184">
-        <v>0.12049851899967801</v>
+        <v>0.18742098038980617</v>
       </c>
       <c r="L184">
         <v>0</v>
       </c>
       <c r="M184">
-        <v>0.22782175671685601</v>
+        <v>0.46011136548279569</v>
       </c>
       <c r="N184">
         <v>0</v>
       </c>
       <c r="O184">
-        <v>4.8791799471685291</v>
+        <v>4.1540560350051585</v>
       </c>
     </row>
     <row r="185" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A185" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B185">
-        <v>46.21755826388241</v>
+        <v>47.246995193818996</v>
       </c>
       <c r="C185">
-        <v>1.8551334779896211</v>
+        <v>1.2374284729159515</v>
       </c>
       <c r="D185">
         <v>0</v>
@@ -9687,39 +9687,39 @@
         <v>0</v>
       </c>
       <c r="H185">
-        <v>2.0743997343479981</v>
+        <v>2.2284017234491982</v>
       </c>
       <c r="I185">
-        <v>0.35315276067282059</v>
+        <v>0.56039000098141933</v>
       </c>
       <c r="J185">
-        <v>0.22087448275496138</v>
+        <v>0.31324000295360593</v>
       </c>
       <c r="K185">
-        <v>0.18742098038980617</v>
+        <v>0.21531220831355802</v>
       </c>
       <c r="L185">
-        <v>0</v>
+        <v>0.15620397198049468</v>
       </c>
       <c r="M185">
-        <v>0.46011136548279569</v>
+        <v>0.61828569032542791</v>
       </c>
       <c r="N185">
         <v>0</v>
       </c>
       <c r="O185">
-        <v>4.1540560350051585</v>
+        <v>3.6847759895374477</v>
       </c>
     </row>
     <row r="186" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A186" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B186">
-        <v>47.246995193818996</v>
+        <v>0</v>
       </c>
       <c r="C186">
-        <v>1.2374284729159515</v>
+        <v>0</v>
       </c>
       <c r="D186">
         <v>0</v>
@@ -9734,33 +9734,33 @@
         <v>0</v>
       </c>
       <c r="H186">
-        <v>2.2284017234491982</v>
+        <v>0</v>
       </c>
       <c r="I186">
-        <v>0.56039000098141933</v>
+        <v>0</v>
       </c>
       <c r="J186">
-        <v>0.31324000295360593</v>
+        <v>0</v>
       </c>
       <c r="K186">
-        <v>0.21531220831355802</v>
+        <v>0</v>
       </c>
       <c r="L186">
-        <v>0.15620397198049468</v>
+        <v>0</v>
       </c>
       <c r="M186">
-        <v>0.61828569032542791</v>
+        <v>0</v>
       </c>
       <c r="N186">
         <v>0</v>
       </c>
       <c r="O186">
-        <v>3.6847759895374477</v>
+        <v>0.17261101503271992</v>
       </c>
     </row>
     <row r="187" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B187">
         <v>0</v>
@@ -9802,15 +9802,15 @@
         <v>0</v>
       </c>
       <c r="O187">
-        <v>0.17261101503271992</v>
+        <v>0.28971753169968123</v>
       </c>
     </row>
     <row r="188" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A188" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B188">
-        <v>0</v>
+        <v>31.472726540678195</v>
       </c>
       <c r="C188">
         <v>0</v>
@@ -9849,18 +9849,18 @@
         <v>0</v>
       </c>
       <c r="O188">
-        <v>0.28971753169968123</v>
+        <v>0.43997864396026309</v>
       </c>
     </row>
     <row r="189" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A189" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B189">
-        <v>31.472726540678195</v>
+        <v>32.25118928408196</v>
       </c>
       <c r="C189">
-        <v>0</v>
+        <v>2.0277086977635552E-2</v>
       </c>
       <c r="D189">
         <v>0</v>
@@ -9875,7 +9875,7 @@
         <v>0</v>
       </c>
       <c r="H189">
-        <v>0</v>
+        <v>0.36288008448910852</v>
       </c>
       <c r="I189">
         <v>0</v>
@@ -9896,18 +9896,18 @@
         <v>0</v>
       </c>
       <c r="O189">
-        <v>0.43997864396026309</v>
+        <v>0.88152069682362999</v>
       </c>
     </row>
     <row r="190" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A190" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B190">
-        <v>32.25118928408196</v>
+        <v>28.897091935211968</v>
       </c>
       <c r="C190">
-        <v>2.0277086977635552E-2</v>
+        <v>0.12955086023569301</v>
       </c>
       <c r="D190">
         <v>0</v>
@@ -9922,7 +9922,7 @@
         <v>0</v>
       </c>
       <c r="H190">
-        <v>0.36288008448910852</v>
+        <v>0.59183780368507899</v>
       </c>
       <c r="I190">
         <v>0</v>
@@ -9943,18 +9943,18 @@
         <v>0</v>
       </c>
       <c r="O190">
-        <v>0.88152069682362999</v>
+        <v>1.6045460155334743</v>
       </c>
     </row>
     <row r="191" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A191" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B191">
-        <v>28.897091935211968</v>
+        <v>24.385675999767052</v>
       </c>
       <c r="C191">
-        <v>0.12955086023569301</v>
+        <v>0.32957914704435542</v>
       </c>
       <c r="D191">
         <v>0</v>
@@ -9969,7 +9969,7 @@
         <v>0</v>
       </c>
       <c r="H191">
-        <v>0.59183780368507899</v>
+        <v>0.91306520098004151</v>
       </c>
       <c r="I191">
         <v>0</v>
@@ -9990,18 +9990,18 @@
         <v>0</v>
       </c>
       <c r="O191">
-        <v>1.6045460155334743</v>
+        <v>2.7482141935452558</v>
       </c>
     </row>
     <row r="192" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A192" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B192">
-        <v>24.385675999767052</v>
+        <v>20.154225663343905</v>
       </c>
       <c r="C192">
-        <v>0.32957914704435542</v>
+        <v>2.2009329928796837</v>
       </c>
       <c r="D192">
         <v>0</v>
@@ -10016,39 +10016,39 @@
         <v>0</v>
       </c>
       <c r="H192">
-        <v>0.91306520098004151</v>
+        <v>0.99871667878189552</v>
       </c>
       <c r="I192">
         <v>0</v>
       </c>
       <c r="J192">
-        <v>0</v>
+        <v>0.18023289885861621</v>
       </c>
       <c r="K192">
-        <v>0</v>
+        <v>0.11059826005601686</v>
       </c>
       <c r="L192">
         <v>0</v>
       </c>
       <c r="M192">
-        <v>0</v>
+        <v>0.1153712820957727</v>
       </c>
       <c r="N192">
         <v>0</v>
       </c>
       <c r="O192">
-        <v>2.7482141935452558</v>
+        <v>3.8226896167542002</v>
       </c>
     </row>
     <row r="193" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B193">
-        <v>20.154225663343905</v>
+        <v>55.871054477305634</v>
       </c>
       <c r="C193">
-        <v>2.2009329928796837</v>
+        <v>2.2892079472910725</v>
       </c>
       <c r="D193">
         <v>0</v>
@@ -10063,39 +10063,39 @@
         <v>0</v>
       </c>
       <c r="H193">
-        <v>0.99871667878189552</v>
+        <v>1.1771465431440027</v>
       </c>
       <c r="I193">
-        <v>0</v>
+        <v>5.2857323993215521E-2</v>
       </c>
       <c r="J193">
-        <v>0.18023289885861621</v>
+        <v>0.19105532429335412</v>
       </c>
       <c r="K193">
-        <v>0.11059826005601686</v>
+        <v>0.10914556053477255</v>
       </c>
       <c r="L193">
         <v>0</v>
       </c>
       <c r="M193">
-        <v>0.1153712820957727</v>
+        <v>7.9577475710236087E-2</v>
       </c>
       <c r="N193">
         <v>0</v>
       </c>
       <c r="O193">
-        <v>3.8226896167542002</v>
+        <v>3.8459377758916378</v>
       </c>
     </row>
     <row r="194" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B194">
-        <v>55.871054477305634</v>
+        <v>43.816543767660242</v>
       </c>
       <c r="C194">
-        <v>2.2892079472910725</v>
+        <v>2.9758908519384231</v>
       </c>
       <c r="D194">
         <v>0</v>
@@ -10110,39 +10110,39 @@
         <v>0</v>
       </c>
       <c r="H194">
-        <v>1.1771465431440027</v>
+        <v>1.3509713570173101</v>
       </c>
       <c r="I194">
-        <v>5.2857323993215521E-2</v>
+        <v>0.20697361160318489</v>
       </c>
       <c r="J194">
-        <v>0.19105532429335412</v>
+        <v>0.28727032601998298</v>
       </c>
       <c r="K194">
-        <v>0.10914556053477255</v>
+        <v>0.20538777577806824</v>
       </c>
       <c r="L194">
-        <v>0</v>
+        <v>0.21104183805035456</v>
       </c>
       <c r="M194">
-        <v>7.9577475710236087E-2</v>
+        <v>0.26649519386978227</v>
       </c>
       <c r="N194">
         <v>0</v>
       </c>
       <c r="O194">
-        <v>3.8459377758916378</v>
+        <v>3.8759988120263404</v>
       </c>
     </row>
     <row r="195" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B195">
-        <v>43.816543767660242</v>
+        <v>45.630878852307454</v>
       </c>
       <c r="C195">
-        <v>2.9758908519384231</v>
+        <v>2.8920319519955546</v>
       </c>
       <c r="D195">
         <v>0</v>
@@ -10157,39 +10157,39 @@
         <v>0</v>
       </c>
       <c r="H195">
-        <v>1.3509713570173101</v>
+        <v>1.9662366016695687</v>
       </c>
       <c r="I195">
-        <v>0.20697361160318489</v>
+        <v>0.37234550549106332</v>
       </c>
       <c r="J195">
-        <v>0.28727032601998298</v>
+        <v>0.51338679852554636</v>
       </c>
       <c r="K195">
-        <v>0.20538777577806824</v>
+        <v>0.26252518074207654</v>
       </c>
       <c r="L195">
-        <v>0.21104183805035456</v>
+        <v>0.31115991053930031</v>
       </c>
       <c r="M195">
-        <v>0.26649519386978227</v>
+        <v>0.67559057446953263</v>
       </c>
       <c r="N195">
         <v>0</v>
       </c>
       <c r="O195">
-        <v>3.8759988120263404</v>
+        <v>4.309191727635227</v>
       </c>
     </row>
     <row r="196" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B196">
-        <v>45.630878852307454</v>
+        <v>47.988593521116535</v>
       </c>
       <c r="C196">
-        <v>2.8920319519955546</v>
+        <v>1.7356245141872702</v>
       </c>
       <c r="D196">
         <v>0</v>
@@ -10204,39 +10204,39 @@
         <v>0</v>
       </c>
       <c r="H196">
-        <v>1.9662366016695687</v>
+        <v>2.4592158224115721</v>
       </c>
       <c r="I196">
-        <v>0.37234550549106332</v>
+        <v>0.42606201804089017</v>
       </c>
       <c r="J196">
-        <v>0.51338679852554636</v>
+        <v>0.53260454256173861</v>
       </c>
       <c r="K196">
-        <v>0.26252518074207654</v>
+        <v>0.33025627131012353</v>
       </c>
       <c r="L196">
-        <v>0.31115991053930031</v>
+        <v>0.4767965521286498</v>
       </c>
       <c r="M196">
-        <v>0.67559057446953263</v>
+        <v>0.84683499811355145</v>
       </c>
       <c r="N196">
         <v>0</v>
       </c>
       <c r="O196">
-        <v>4.309191727635227</v>
+        <v>3.7634164215770829</v>
       </c>
     </row>
     <row r="197" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B197">
-        <v>47.988593521116535</v>
+        <v>0</v>
       </c>
       <c r="C197">
-        <v>1.7356245141872702</v>
+        <v>0</v>
       </c>
       <c r="D197">
         <v>0</v>
@@ -10251,33 +10251,33 @@
         <v>0</v>
       </c>
       <c r="H197">
-        <v>2.4592158224115721</v>
+        <v>0</v>
       </c>
       <c r="I197">
-        <v>0.42606201804089017</v>
+        <v>0</v>
       </c>
       <c r="J197">
-        <v>0.53260454256173861</v>
+        <v>0</v>
       </c>
       <c r="K197">
-        <v>0.33025627131012353</v>
+        <v>0</v>
       </c>
       <c r="L197">
-        <v>0.4767965521286498</v>
+        <v>0</v>
       </c>
       <c r="M197">
-        <v>0.84683499811355145</v>
+        <v>0</v>
       </c>
       <c r="N197">
         <v>0</v>
       </c>
       <c r="O197">
-        <v>3.7634164215770829</v>
+        <v>0.18912118656579155</v>
       </c>
     </row>
     <row r="198" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B198">
         <v>0</v>
@@ -10319,15 +10319,15 @@
         <v>0</v>
       </c>
       <c r="O198">
-        <v>0.18912118656579155</v>
+        <v>0.3016162993495049</v>
       </c>
     </row>
     <row r="199" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B199">
-        <v>0</v>
+        <v>30.71722205423734</v>
       </c>
       <c r="C199">
         <v>0</v>
@@ -10366,18 +10366,18 @@
         <v>0</v>
       </c>
       <c r="O199">
-        <v>0.3016162993495049</v>
+        <v>0.5922641009594678</v>
       </c>
     </row>
     <row r="200" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B200">
-        <v>30.71722205423734</v>
+        <v>28.073410006153523</v>
       </c>
       <c r="C200">
-        <v>0</v>
+        <v>3.0803275535077113E-2</v>
       </c>
       <c r="D200">
         <v>0</v>
@@ -10392,7 +10392,7 @@
         <v>0</v>
       </c>
       <c r="H200">
-        <v>0</v>
+        <v>0.41926266621775354</v>
       </c>
       <c r="I200">
         <v>0</v>
@@ -10413,18 +10413,18 @@
         <v>0</v>
       </c>
       <c r="O200">
-        <v>0.5922641009594678</v>
+        <v>1.1816937731692321</v>
       </c>
     </row>
     <row r="201" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B201">
-        <v>28.073410006153523</v>
+        <v>26.381952311914045</v>
       </c>
       <c r="C201">
-        <v>3.0803275535077113E-2</v>
+        <v>0.18953931778532318</v>
       </c>
       <c r="D201">
         <v>0</v>
@@ -10439,7 +10439,7 @@
         <v>0</v>
       </c>
       <c r="H201">
-        <v>0.41926266621775354</v>
+        <v>0.66511866970724265</v>
       </c>
       <c r="I201">
         <v>0</v>
@@ -10460,18 +10460,18 @@
         <v>0</v>
       </c>
       <c r="O201">
-        <v>1.1816937731692321</v>
+        <v>2.0753642015315914</v>
       </c>
     </row>
     <row r="202" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B202">
-        <v>26.381952311914045</v>
+        <v>25.045296948273563</v>
       </c>
       <c r="C202">
-        <v>0.18953931778532318</v>
+        <v>0.43940395617208799</v>
       </c>
       <c r="D202">
         <v>0</v>
@@ -10486,13 +10486,13 @@
         <v>0</v>
       </c>
       <c r="H202">
-        <v>0.66511866970724265</v>
+        <v>0.91293844493479281</v>
       </c>
       <c r="I202">
         <v>0</v>
       </c>
       <c r="J202">
-        <v>0</v>
+        <v>0.11202242405095937</v>
       </c>
       <c r="K202">
         <v>0</v>
@@ -10507,18 +10507,18 @@
         <v>0</v>
       </c>
       <c r="O202">
-        <v>2.0753642015315914</v>
+        <v>3.4673153872867575</v>
       </c>
     </row>
     <row r="203" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B203">
-        <v>25.045296948273563</v>
+        <v>21.762418838575016</v>
       </c>
       <c r="C203">
-        <v>0.43940395617208799</v>
+        <v>1.2233611120423036</v>
       </c>
       <c r="D203">
         <v>0</v>
@@ -10533,39 +10533,39 @@
         <v>0</v>
       </c>
       <c r="H203">
-        <v>0.91293844493479281</v>
+        <v>1.214030853467944</v>
       </c>
       <c r="I203">
         <v>0</v>
       </c>
       <c r="J203">
-        <v>0.11202242405095937</v>
+        <v>0.10424138322565431</v>
       </c>
       <c r="K203">
-        <v>0</v>
+        <v>0.22817472397633792</v>
       </c>
       <c r="L203">
-        <v>0</v>
+        <v>0.20567206691260745</v>
       </c>
       <c r="M203">
-        <v>0</v>
+        <v>8.4189473276039331E-2</v>
       </c>
       <c r="N203">
         <v>0</v>
       </c>
       <c r="O203">
-        <v>3.4673153872867575</v>
+        <v>4.5693894288319381</v>
       </c>
     </row>
     <row r="204" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B204">
-        <v>21.762418838575016</v>
+        <v>56.33283154570185</v>
       </c>
       <c r="C204">
-        <v>1.2233611120423036</v>
+        <v>1.3553468317047028</v>
       </c>
       <c r="D204">
         <v>0</v>
@@ -10580,39 +10580,39 @@
         <v>0</v>
       </c>
       <c r="H204">
-        <v>1.214030853467944</v>
+        <v>1.101350214213054</v>
       </c>
       <c r="I204">
-        <v>0</v>
+        <v>4.2087376212465673E-2</v>
       </c>
       <c r="J204">
-        <v>0.10424138322565431</v>
+        <v>0.32505542545760785</v>
       </c>
       <c r="K204">
-        <v>0.22817472397633792</v>
+        <v>0.13721191055932067</v>
       </c>
       <c r="L204">
-        <v>0.20567206691260745</v>
+        <v>0.21879276888309881</v>
       </c>
       <c r="M204">
-        <v>8.4189473276039331E-2</v>
+        <v>0</v>
       </c>
       <c r="N204">
         <v>0</v>
       </c>
       <c r="O204">
-        <v>4.5693894288319381</v>
+        <v>4.366179617970336</v>
       </c>
     </row>
     <row r="205" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B205">
-        <v>56.33283154570185</v>
+        <v>48.916254618077204</v>
       </c>
       <c r="C205">
-        <v>1.3553468317047028</v>
+        <v>1.2737925974662152</v>
       </c>
       <c r="D205">
         <v>0</v>
@@ -10627,39 +10627,39 @@
         <v>0</v>
       </c>
       <c r="H205">
-        <v>1.101350214213054</v>
+        <v>1.2043134272409395</v>
       </c>
       <c r="I205">
-        <v>4.2087376212465673E-2</v>
+        <v>0.16195263216014352</v>
       </c>
       <c r="J205">
-        <v>0.32505542545760785</v>
+        <v>0.39219481207733198</v>
       </c>
       <c r="K205">
-        <v>0.13721191055932067</v>
+        <v>0.3009883711507868</v>
       </c>
       <c r="L205">
-        <v>0.21879276888309881</v>
+        <v>0.44396369146214665</v>
       </c>
       <c r="M205">
-        <v>0</v>
+        <v>0.19471997334958671</v>
       </c>
       <c r="N205">
         <v>0</v>
       </c>
       <c r="O205">
-        <v>4.366179617970336</v>
+        <v>4.522060750442594</v>
       </c>
     </row>
     <row r="206" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A206" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B206">
-        <v>48.916254618077204</v>
+        <v>52.28496147586813</v>
       </c>
       <c r="C206">
-        <v>1.2737925974662152</v>
+        <v>0.71854627416972372</v>
       </c>
       <c r="D206">
         <v>0</v>
@@ -10674,39 +10674,39 @@
         <v>0</v>
       </c>
       <c r="H206">
-        <v>1.2043134272409395</v>
+        <v>1.2998182287158897</v>
       </c>
       <c r="I206">
-        <v>0.16195263216014352</v>
+        <v>0.26729175023664231</v>
       </c>
       <c r="J206">
-        <v>0.39219481207733198</v>
+        <v>0.44931189297059793</v>
       </c>
       <c r="K206">
-        <v>0.3009883711507868</v>
+        <v>0.3959185423599948</v>
       </c>
       <c r="L206">
-        <v>0.44396369146214665</v>
+        <v>0.89179514276963046</v>
       </c>
       <c r="M206">
-        <v>0.19471997334958671</v>
+        <v>0.43046814723809879</v>
       </c>
       <c r="N206">
         <v>0</v>
       </c>
       <c r="O206">
-        <v>4.522060750442594</v>
+        <v>3.9445052514132342</v>
       </c>
     </row>
     <row r="207" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A207" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B207">
-        <v>52.28496147586813</v>
+        <v>48.814065435851816</v>
       </c>
       <c r="C207">
-        <v>0.71854627416972372</v>
+        <v>0.37730400981341072</v>
       </c>
       <c r="D207">
         <v>0</v>
@@ -10721,79 +10721,33 @@
         <v>0</v>
       </c>
       <c r="H207">
-        <v>1.2998182287158897</v>
+        <v>1.3686017082429383</v>
       </c>
       <c r="I207">
-        <v>0.26729175023664231</v>
+        <v>0.24591115913729458</v>
       </c>
       <c r="J207">
-        <v>0.44931189297059793</v>
+        <v>0.50770737080541706</v>
       </c>
       <c r="K207">
-        <v>0.3959185423599948</v>
+        <v>0.51635186646277198</v>
       </c>
       <c r="L207">
-        <v>0.89179514276963046</v>
+        <v>0.86574385461561854</v>
       </c>
       <c r="M207">
-        <v>0.43046814723809879</v>
+        <v>0.91745650805223644</v>
       </c>
       <c r="N207">
         <v>0</v>
       </c>
       <c r="O207">
-        <v>3.9445052514132342</v>
-      </c>
-    </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A208" t="s">
-        <v>221</v>
-      </c>
-      <c r="B208">
-        <v>48.814065435851816</v>
-      </c>
-      <c r="C208">
-        <v>0.37730400981341072</v>
-      </c>
-      <c r="D208">
-        <v>0</v>
-      </c>
-      <c r="E208">
-        <v>0</v>
-      </c>
-      <c r="F208">
-        <v>0</v>
-      </c>
-      <c r="G208">
-        <v>0</v>
-      </c>
-      <c r="H208">
-        <v>1.3686017082429383</v>
-      </c>
-      <c r="I208">
-        <v>0.24591115913729458</v>
-      </c>
-      <c r="J208">
-        <v>0.50770737080541706</v>
-      </c>
-      <c r="K208">
-        <v>0.51635186646277198</v>
-      </c>
-      <c r="L208">
-        <v>0.86574385461561854</v>
-      </c>
-      <c r="M208">
-        <v>0.91745650805223644</v>
-      </c>
-      <c r="N208">
-        <v>0</v>
-      </c>
-      <c r="O208">
         <v>4.3433607179449378</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 

</xml_diff>